<commit_message>
Contact Us Page Implemented
2020/03/24
</commit_message>
<xml_diff>
--- a/src/test/java/ExcelFiles/tollPaysAppKeywords.xlsx
+++ b/src/test/java/ExcelFiles/tollPaysAppKeywords.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="330" yWindow="330" windowWidth="18000" windowHeight="9480" activeTab="1"/>
+    <workbookView xWindow="330" yWindow="330" windowWidth="18000" windowHeight="9480" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sign In Module" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -83,10 +83,34 @@
     <t>//a[contains(text(),'Contact Us')]</t>
   </si>
   <si>
-    <t>Contact Us Button</t>
-  </si>
-  <si>
-    <t>Submit Button</t>
+    <t>//select[@id='subject']</t>
+  </si>
+  <si>
+    <t>//select[@id='account_type']</t>
+  </si>
+  <si>
+    <t>account_type</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>//input[@id='email']</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>//textarea[@id='message']</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>contact_us</t>
+  </si>
+  <si>
+    <t>submit</t>
   </si>
 </sst>
 </file>
@@ -524,7 +548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -627,17 +651,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -656,7 +681,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -666,19 +691,61 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified Sign In Screen with DDD Framework!
2020/03/29
</commit_message>
<xml_diff>
--- a/src/test/java/ExcelFiles/tollPaysAppKeywords.xlsx
+++ b/src/test/java/ExcelFiles/tollPaysAppKeywords.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>ID</t>
   </si>
@@ -56,15 +56,6 @@
     <t>Sign In Button</t>
   </si>
   <si>
-    <t>//*[@id="doLogin"]/div[2]/div[1]/input</t>
-  </si>
-  <si>
-    <t>//*[@id="doLogin"]/div[2]/div[2]/input</t>
-  </si>
-  <si>
-    <t>//*[@id="doLogin"]/div[2]/div[4]/div/button</t>
-  </si>
-  <si>
     <t>//a[contains(text(),'Sign Up')]</t>
   </si>
   <si>
@@ -126,6 +117,36 @@
   </si>
   <si>
     <t>Please respond ASAP!</t>
+  </si>
+  <si>
+    <t>email address</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>stayseated05@gmail.com</t>
+  </si>
+  <si>
+    <t>1111111A</t>
+  </si>
+  <si>
+    <t>Sign In Submit Button</t>
+  </si>
+  <si>
+    <t>button_signin</t>
+  </si>
+  <si>
+    <t>loginid</t>
+  </si>
+  <si>
+    <t>//input[@id='password']</t>
+  </si>
+  <si>
+    <t>//input[@id='loginid']</t>
+  </si>
+  <si>
+    <t>//button[@class='btn btn-primary smtBtn ajax']</t>
   </si>
 </sst>
 </file>
@@ -508,20 +529,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -534,40 +559,71 @@
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -602,22 +658,22 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -681,7 +737,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,67 +764,67 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -777,7 +833,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -785,18 +841,18 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>